<commit_message>
分支：dyt_targetApi31_0825 Module： 版本：VersionName:1.4.01 , VersionCode:230 合并224，1.3.14版本的业务逻辑 之前备份。 上传时间：2022年9月27日11:24:25
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="19005" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="SN区分表" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="271">
   <si>
     <t>使用公司</t>
   </si>
@@ -35,6 +35,12 @@
     <t>机芯分辨率</t>
   </si>
   <si>
+    <t>客户型号</t>
+  </si>
+  <si>
+    <t>型号密文（本地保存：）</t>
+  </si>
+  <si>
     <t>备注</t>
   </si>
   <si>
@@ -98,6 +104,12 @@
     <t>256*192</t>
   </si>
   <si>
+    <t>H2F</t>
+  </si>
+  <si>
+    <t>5FxrPF85yybK3mqurm1mXw==</t>
+  </si>
+  <si>
     <t>DYTH200D</t>
   </si>
   <si>
@@ -116,6 +128,12 @@
     <t>160*120</t>
   </si>
   <si>
+    <t>H1F</t>
+  </si>
+  <si>
+    <t>EE6P/0TFDXQbWTj07df+Cg==</t>
+  </si>
+  <si>
     <t>精明鼠</t>
   </si>
   <si>
@@ -125,6 +143,12 @@
     <t>LiAkhdbCnh2rcDlS81+TzQ==</t>
   </si>
   <si>
+    <t>NF-583S</t>
+  </si>
+  <si>
+    <t>nnDIX4TEk8JaOs36tYQiZw==</t>
+  </si>
+  <si>
     <t>LiAkhdbCnh2rcDlS81+TzQ==;8gLNtq/EDcdjmswJNizkRg==</t>
   </si>
   <si>
@@ -134,6 +158,12 @@
     <t>8gLNtq/EDcdjmswJNizkRg==</t>
   </si>
   <si>
+    <t>NF-586S</t>
+  </si>
+  <si>
+    <t>2MrTTGGzrbaUFbfpx9dLFw==</t>
+  </si>
+  <si>
     <t>胜利</t>
   </si>
   <si>
@@ -143,6 +173,12 @@
     <t>sxu3KZt/XNXvXQEnY75I1g==</t>
   </si>
   <si>
+    <t>VICTOR 328A</t>
+  </si>
+  <si>
+    <t>MP0kyCEcW8GqSa3h65jLBg==</t>
+  </si>
+  <si>
     <t>sxu3KZt/XNXvXQEnY75I1g==;Xf3p+bjmiqjkNwTZIEYu7A==</t>
   </si>
   <si>
@@ -152,6 +188,12 @@
     <t>Xf3p+bjmiqjkNwTZIEYu7A==</t>
   </si>
   <si>
+    <t>VICTOR 328B</t>
+  </si>
+  <si>
+    <t>8XvQOcWqgko4LFXrl/A0HA==</t>
+  </si>
+  <si>
     <t>潜力</t>
   </si>
   <si>
@@ -161,6 +203,12 @@
     <t>OnR6llCcnFQx9a7cNQGD0g==</t>
   </si>
   <si>
+    <t>火眼 IR EYE</t>
+  </si>
+  <si>
+    <t>LGwucKSw8Av0siJVdx2zoA==</t>
+  </si>
+  <si>
     <t>泰视朗</t>
   </si>
   <si>
@@ -188,6 +236,12 @@
     <t>obecpV08fDdHzlnPOZhIqg==</t>
   </si>
   <si>
+    <t>TR160</t>
+  </si>
+  <si>
+    <t>xPf7qTfvvfxyTCeUGrZgjA==</t>
+  </si>
+  <si>
     <t>obecpV08fDdHzlnPOZhIqg==;RHRhyWZePEEvIPQg/6Fdrg==</t>
   </si>
   <si>
@@ -200,6 +254,12 @@
     <t>RHRhyWZePEEvIPQg/6Fdrg==</t>
   </si>
   <si>
+    <t>TR256</t>
+  </si>
+  <si>
+    <t>iCEAJFzcyKpSk7xxoaaivg==</t>
+  </si>
+  <si>
     <t>光智</t>
   </si>
   <si>
@@ -209,6 +269,12 @@
     <t>h8YZ6js1ZBdbtDLA1v3KYw==</t>
   </si>
   <si>
+    <t>VOT-SP1A</t>
+  </si>
+  <si>
+    <t>t/aG12Ku8lcMXjvL0IKlDw==</t>
+  </si>
+  <si>
     <t>h8YZ6js1ZBdbtDLA1v3KYw==;jXDHHhEgRee3USPxO7C+oA==</t>
   </si>
   <si>
@@ -218,6 +284,12 @@
     <t>jXDHHhEgRee3USPxO7C+oA==</t>
   </si>
   <si>
+    <t>VOT-SP1B</t>
+  </si>
+  <si>
+    <t>KHDcDaovivPG8LTvXRskUA==</t>
+  </si>
+  <si>
     <t>睿迪菲尔</t>
   </si>
   <si>
@@ -225,6 +297,12 @@
   </si>
   <si>
     <t>fCH2xUWvp0qNowOdVQ05XQ==</t>
+  </si>
+  <si>
+    <t>RF2</t>
+  </si>
+  <si>
+    <t>Dj8D7J6Nwzh/UH5kw0PcMQ==</t>
   </si>
   <si>
     <t>软件包名</t>
@@ -2311,10 +2389,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -2386,21 +2464,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -2408,23 +2472,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2438,7 +2495,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2446,24 +2510,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2485,11 +2541,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2502,15 +2595,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2518,13 +2603,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2551,7 +2629,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2563,37 +2767,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2605,115 +2779,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2731,7 +2809,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2847,30 +2925,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2878,21 +2932,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2906,17 +2945,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,6 +2977,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2952,10 +3030,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2964,133 +3042,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3965,24 +4043,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="32" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="32" customWidth="1"/>
-    <col min="4" max="4" width="27.625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="25.375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="30" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="32"/>
+    <col min="1" max="1" width="18" style="32" customWidth="1"/>
+    <col min="2" max="2" width="14.625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="29.875" style="32" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="14.75" style="32" customWidth="1"/>
+    <col min="6" max="6" width="20" style="32" customWidth="1"/>
+    <col min="7" max="7" width="27" style="32" customWidth="1"/>
+    <col min="8" max="8" width="30" style="32" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:17">
+    <row r="1" customHeight="1" spans="1:19">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -4001,35 +4081,41 @@
       <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
-    <row r="2" customHeight="1" spans="1:17">
+    <row r="2" customHeight="1" spans="1:19">
       <c r="A2" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="F2" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="29" t="s">
+        <v>11</v>
+      </c>
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
@@ -4039,21 +4125,23 @@
       <c r="O2" s="29"/>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
-    <row r="3" customHeight="1" spans="1:17">
+    <row r="3" customHeight="1" spans="1:19">
       <c r="A3" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
@@ -4064,21 +4152,23 @@
       <c r="O3" s="29"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
-    <row r="4" customHeight="1" spans="1:17">
+    <row r="4" customHeight="1" spans="1:19">
       <c r="A4" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
@@ -4089,21 +4179,23 @@
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
     </row>
-    <row r="5" customHeight="1" spans="1:17">
+    <row r="5" customHeight="1" spans="1:19">
       <c r="A5" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
@@ -4114,21 +4206,23 @@
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
     </row>
-    <row r="6" customHeight="1" spans="1:17">
+    <row r="6" customHeight="1" spans="1:19">
       <c r="A6" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
@@ -4139,21 +4233,23 @@
       <c r="O6" s="29"/>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
     </row>
-    <row r="7" customHeight="1" spans="1:17">
+    <row r="7" customHeight="1" spans="1:19">
       <c r="A7" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
@@ -4164,21 +4260,23 @@
       <c r="O7" s="29"/>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
     </row>
-    <row r="8" customHeight="1" spans="1:17">
+    <row r="8" customHeight="1" spans="1:19">
       <c r="A8" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
@@ -4189,25 +4287,31 @@
       <c r="O8" s="29"/>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
     </row>
-    <row r="9" customHeight="1" spans="1:17">
+    <row r="9" customHeight="1" spans="1:19">
       <c r="A9" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -4218,25 +4322,27 @@
       <c r="O9" s="29"/>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
     </row>
-    <row r="10" customHeight="1" spans="1:17">
+    <row r="10" customHeight="1" spans="1:19">
       <c r="A10" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
@@ -4247,25 +4353,31 @@
       <c r="O10" s="29"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
     </row>
-    <row r="11" customHeight="1" spans="1:17">
+    <row r="11" customHeight="1" spans="1:19">
       <c r="A11" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
@@ -4276,21 +4388,23 @@
       <c r="O11" s="29"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
     </row>
-    <row r="12" customHeight="1" spans="1:17">
+    <row r="12" customHeight="1" spans="1:19">
       <c r="A12" s="20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
@@ -4301,15 +4415,17 @@
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
     </row>
-    <row r="13" customHeight="1" spans="1:17">
+    <row r="13" customHeight="1" spans="1:19">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
@@ -4320,15 +4436,17 @@
       <c r="O13" s="29"/>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
     </row>
-    <row r="14" customHeight="1" spans="1:17">
+    <row r="14" customHeight="1" spans="1:19">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
@@ -4339,15 +4457,17 @@
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
     </row>
-    <row r="15" customHeight="1" spans="1:17">
+    <row r="15" customHeight="1" spans="1:19">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
       <c r="J15" s="29"/>
@@ -4358,28 +4478,34 @@
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
     </row>
-    <row r="16" customHeight="1" spans="1:17">
+    <row r="16" customHeight="1" spans="1:19">
       <c r="A16" s="20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="F16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>43</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
@@ -4389,25 +4515,31 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
     </row>
-    <row r="17" customHeight="1" spans="1:17">
+    <row r="17" customHeight="1" spans="1:19">
       <c r="A17" s="20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>47</v>
+      </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -4418,15 +4550,17 @@
       <c r="O17" s="29"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
     </row>
-    <row r="18" customHeight="1" spans="1:17">
+    <row r="18" customHeight="1" spans="1:19">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
@@ -4437,15 +4571,17 @@
       <c r="O18" s="29"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
     </row>
-    <row r="19" customHeight="1" spans="1:17">
+    <row r="19" customHeight="1" spans="1:19">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
@@ -4456,42 +4592,50 @@
       <c r="O19" s="29"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
     </row>
-    <row r="20" customHeight="1" spans="1:17">
+    <row r="20" customHeight="1" spans="1:19">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
       <c r="M20" s="29"/>
       <c r="N20" s="29"/>
       <c r="O20" s="29"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
     </row>
-    <row r="21" customHeight="1" spans="1:17">
+    <row r="21" customHeight="1" spans="1:19">
       <c r="A21" s="20" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>53</v>
+      </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
@@ -4501,25 +4645,31 @@
       <c r="O21" s="29"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
     </row>
-    <row r="22" customHeight="1" spans="1:17">
+    <row r="22" customHeight="1" spans="1:19">
       <c r="A22" s="20" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
@@ -4530,15 +4680,17 @@
       <c r="O22" s="29"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
     </row>
-    <row r="23" customHeight="1" spans="1:17">
+    <row r="23" customHeight="1" spans="1:19">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
@@ -4549,26 +4701,32 @@
       <c r="O23" s="29"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
     </row>
-    <row r="24" customHeight="1" spans="1:17">
+    <row r="24" customHeight="1" spans="1:19">
       <c r="A24" s="20" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
+      <c r="F24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
@@ -4578,15 +4736,17 @@
       <c r="O24" s="29"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
     </row>
-    <row r="25" customHeight="1" spans="1:17">
+    <row r="25" customHeight="1" spans="1:19">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -4597,15 +4757,17 @@
       <c r="O25" s="29"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
     </row>
-    <row r="26" customHeight="1" spans="1:17">
+    <row r="26" customHeight="1" spans="1:19">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
@@ -4616,15 +4778,17 @@
       <c r="O26" s="29"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
     </row>
-    <row r="27" customHeight="1" spans="1:17">
+    <row r="27" customHeight="1" spans="1:19">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
@@ -4635,28 +4799,30 @@
       <c r="O27" s="29"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
     </row>
-    <row r="28" customHeight="1" spans="1:17">
+    <row r="28" customHeight="1" spans="1:19">
       <c r="A28" s="20" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
@@ -4666,25 +4832,27 @@
       <c r="O28" s="29"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
     </row>
-    <row r="29" customHeight="1" spans="1:17">
+    <row r="29" customHeight="1" spans="1:19">
       <c r="A29" s="20" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
@@ -4695,15 +4863,17 @@
       <c r="O29" s="29"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
     </row>
-    <row r="30" customHeight="1" spans="1:17">
+    <row r="30" customHeight="1" spans="1:19">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
@@ -4714,28 +4884,34 @@
       <c r="O30" s="29"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
     </row>
-    <row r="31" customHeight="1" spans="1:17">
+    <row r="31" customHeight="1" spans="1:19">
       <c r="A31" s="20" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>74</v>
+      </c>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
@@ -4745,25 +4921,31 @@
       <c r="O31" s="29"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
     </row>
-    <row r="32" customHeight="1" spans="1:17">
+    <row r="32" customHeight="1" spans="1:19">
       <c r="A32" s="20" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
@@ -4774,15 +4956,17 @@
       <c r="O32" s="29"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
     </row>
-    <row r="33" customHeight="1" spans="1:17">
+    <row r="33" customHeight="1" spans="1:19">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
       <c r="J33" s="29"/>
@@ -4793,28 +4977,34 @@
       <c r="O33" s="29"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
     </row>
-    <row r="34" customHeight="1" spans="1:17">
+    <row r="34" customHeight="1" spans="1:19">
       <c r="A34" s="20" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="I34" s="29"/>
       <c r="J34" s="29"/>
       <c r="K34" s="29"/>
@@ -4824,25 +5014,31 @@
       <c r="O34" s="29"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
     </row>
-    <row r="35" customHeight="1" spans="1:17">
+    <row r="35" customHeight="1" spans="1:19">
       <c r="A35" s="20" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
       <c r="J35" s="29"/>
@@ -4853,15 +5049,17 @@
       <c r="O35" s="29"/>
       <c r="P35" s="29"/>
       <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
     </row>
-    <row r="36" customHeight="1" spans="1:17">
+    <row r="36" customHeight="1" spans="1:19">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
@@ -4872,28 +5070,34 @@
       <c r="O36" s="29"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
     </row>
-    <row r="37" customHeight="1" spans="1:17">
+    <row r="37" customHeight="1" spans="1:19">
       <c r="A37" s="20" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>92</v>
+      </c>
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
@@ -4903,15 +5107,17 @@
       <c r="O37" s="29"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
     </row>
-    <row r="38" customHeight="1" spans="1:17">
+    <row r="38" customHeight="1" spans="1:19">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
       <c r="J38" s="29"/>
@@ -4922,15 +5128,17 @@
       <c r="O38" s="29"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
     </row>
-    <row r="39" customHeight="1" spans="1:17">
+    <row r="39" customHeight="1" spans="1:19">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
@@ -4941,8 +5149,10 @@
       <c r="O39" s="29"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
     </row>
-    <row r="40" customHeight="1" spans="1:17">
+    <row r="40" customHeight="1" spans="1:19">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -4960,8 +5170,10 @@
       <c r="O40" s="29"/>
       <c r="P40" s="29"/>
       <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
     </row>
-    <row r="41" customHeight="1" spans="1:17">
+    <row r="41" customHeight="1" spans="1:19">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -4979,8 +5191,10 @@
       <c r="O41" s="29"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
     </row>
-    <row r="42" customHeight="1" spans="1:17">
+    <row r="42" customHeight="1" spans="1:19">
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -4998,8 +5212,10 @@
       <c r="O42" s="29"/>
       <c r="P42" s="29"/>
       <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
     </row>
-    <row r="43" customHeight="1" spans="1:17">
+    <row r="43" customHeight="1" spans="1:19">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -5017,8 +5233,10 @@
       <c r="O43" s="29"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
     </row>
-    <row r="44" customHeight="1" spans="1:17">
+    <row r="44" customHeight="1" spans="1:19">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -5036,8 +5254,10 @@
       <c r="O44" s="29"/>
       <c r="P44" s="29"/>
       <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
     </row>
-    <row r="45" customHeight="1" spans="2:17">
+    <row r="45" customHeight="1" spans="2:19">
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
@@ -5054,8 +5274,10 @@
       <c r="O45" s="29"/>
       <c r="P45" s="29"/>
       <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
     </row>
-    <row r="46" customHeight="1" spans="2:17">
+    <row r="46" customHeight="1" spans="2:19">
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
@@ -5072,8 +5294,10 @@
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
+      <c r="S46" s="29"/>
     </row>
-    <row r="47" customHeight="1" spans="2:17">
+    <row r="47" customHeight="1" spans="2:19">
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
@@ -5090,8 +5314,10 @@
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
     </row>
-    <row r="48" customHeight="1" spans="2:17">
+    <row r="48" customHeight="1" spans="2:19">
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
@@ -5108,17 +5334,19 @@
       <c r="O48" s="29"/>
       <c r="P48" s="29"/>
       <c r="Q48" s="29"/>
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="F37:J37"/>
-    <mergeCell ref="F16:J18"/>
-    <mergeCell ref="F2:J7"/>
-    <mergeCell ref="F21:J22"/>
-    <mergeCell ref="F28:J29"/>
-    <mergeCell ref="F24:J25"/>
-    <mergeCell ref="F31:J32"/>
-    <mergeCell ref="F34:J35"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H16:L18"/>
+    <mergeCell ref="H2:L7"/>
+    <mergeCell ref="H21:L22"/>
+    <mergeCell ref="H28:L29"/>
+    <mergeCell ref="H24:L25"/>
+    <mergeCell ref="H31:L32"/>
+    <mergeCell ref="H34:L35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -5147,22 +5375,22 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:15">
       <c r="A1" s="19" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
@@ -5176,22 +5404,22 @@
     </row>
     <row r="2" customHeight="1" spans="1:16384">
       <c r="A2" s="25" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
@@ -21574,179 +21802,179 @@
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="19" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" ht="39" customHeight="1" spans="1:6">
       <c r="A4" s="19" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="19" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="19" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="19" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="19" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="19" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="29" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="19" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" ht="41" customHeight="1" spans="1:6">
       <c r="A11" s="19" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" ht="31" customHeight="1" spans="1:6">
       <c r="A12" s="19" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="29" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" ht="45" customHeight="1" spans="1:5">
       <c r="A13" s="19" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="30"/>
@@ -21769,7 +21997,7 @@
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="19" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E18" s="30"/>
     </row>
@@ -21809,14 +22037,14 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="21" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="19" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
@@ -21824,32 +22052,32 @@
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="6" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -21858,40 +22086,40 @@
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" customHeight="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="6" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -21911,93 +22139,93 @@
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" customHeight="1" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" customHeight="1" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customHeight="1" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="6" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -22009,58 +22237,58 @@
     </row>
     <row r="17" customHeight="1" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" customHeight="1" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" customHeight="1" spans="1:9">
       <c r="A20" s="7" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="B20" s="7">
         <v>101</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -22069,249 +22297,249 @@
     </row>
     <row r="21" customHeight="1" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="B21" s="7">
         <v>102</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="B22" s="7">
         <v>103</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" customHeight="1" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="B23" s="7">
         <v>104</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="122" customHeight="1" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="B24" s="7">
         <v>105</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" ht="90" customHeight="1" spans="1:4">
       <c r="A25" s="20" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="B25" s="20">
         <v>110</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:4">
       <c r="A26" s="19" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:4">
       <c r="A27" s="19" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="B27" s="19">
         <v>113</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:4">
       <c r="A28" s="19" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="B28" s="19">
         <v>201</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:4">
       <c r="A29" s="19" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="B29" s="19">
         <v>203</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:4">
       <c r="A30" s="19" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="B30" s="19">
         <v>204</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:4">
       <c r="A31" s="19" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="B31" s="19">
         <v>205</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:4">
       <c r="A32" s="19" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="B32" s="19">
         <v>206</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:4">
       <c r="A33" s="19" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="B33" s="19">
         <v>207</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" ht="88" customHeight="1" spans="1:5">
       <c r="A34" s="19" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="B34" s="19">
         <v>208</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" ht="151" customHeight="1" spans="1:4">
       <c r="A35" s="19" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="B35" s="19">
         <v>209</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" ht="101" customHeight="1" spans="1:4">
       <c r="A36" s="19" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="B36" s="19">
         <v>216</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" ht="134" customHeight="1" spans="1:4">
       <c r="A37" s="19" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="B37" s="19">
         <v>217</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -22354,7 +22582,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="15" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -22363,86 +22591,86 @@
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="B3" s="16">
         <v>101</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="F3" s="17"/>
     </row>
     <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="16" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="B4" s="16">
         <v>103</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
     </row>
     <row r="5" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="B5" s="16">
         <v>104</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
     </row>
     <row r="6" ht="81.75" spans="1:6">
       <c r="A6" s="16" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="B6" s="16">
         <v>105</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -22929,7 +23157,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -22938,80 +23166,80 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="B3" s="6">
         <v>101</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="B4" s="6">
         <v>102</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="98" customHeight="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="B5" s="6">
         <v>103</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="B6" s="9">
         <v>104</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -23031,31 +23259,31 @@
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="B9" s="7">
         <v>105</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="E9" s="11"/>
     </row>
     <row r="10" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B10" s="6">
         <v>106</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="E10" s="7"/>
     </row>

</xml_diff>

<commit_message>
分支：dyt_targetApi31_0825 Module： 版本：VersionName:1.4.04 , VersionCode:233 1、已有版本，关于界面增加“型号”。 2、适当调整app logo大小
上传时间：2022年11月3日15:09:04
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -2389,12 +2389,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2464,56 +2464,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="12"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2532,32 +2492,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2571,7 +2514,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2586,15 +2553,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2605,6 +2587,30 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2629,7 +2635,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2641,37 +2725,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2683,133 +2815,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2925,6 +2931,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2945,50 +2960,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3022,6 +2993,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3030,10 +3036,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3042,137 +3048,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3269,6 +3275,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4046,7 +4055,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
@@ -4705,7 +4714,7 @@
       <c r="S23" s="29"/>
     </row>
     <row r="24" customHeight="1" spans="1:19">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -4718,7 +4727,7 @@
         <v>26</v>
       </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="33" t="s">
         <v>61</v>
       </c>
       <c r="G24" s="20" t="s">
@@ -4803,7 +4812,7 @@
       <c r="S27" s="29"/>
     </row>
     <row r="28" customHeight="1" spans="1:19">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="20" t="s">
@@ -4836,7 +4845,7 @@
       <c r="S28" s="29"/>
     </row>
     <row r="29" customHeight="1" spans="1:19">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="20" t="s">

</xml_diff>

<commit_message>
分支：dyt_targetApi31_0825 Module： 版本：VersionName:1.4.06 , VersionCode:235 模块新增，架构调整：MTI448首页调整，备份,图库重整 上传时间：2022年11月24日18:17:30
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="2"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="SN区分表" sheetId="1" r:id="rId1"/>
@@ -2040,9 +2040,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
@@ -2114,6 +2114,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -2128,8 +2143,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2150,15 +2196,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2166,23 +2203,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -2197,21 +2219,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -2221,10 +2228,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2236,23 +2243,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2279,13 +2279,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2297,13 +2309,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2321,19 +2345,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2345,91 +2381,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2447,19 +2405,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2521,17 +2521,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2564,9 +2553,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2590,7 +2599,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2609,15 +2618,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2626,10 +2626,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2638,133 +2638,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3617,8 +3617,8 @@
   <sheetPr/>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
@@ -21649,7 +21649,7 @@
   <sheetPr/>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A37" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
分支：dyt_targetApi31_0825 版本：VersionName:1.5.02 ,VersionCode:252 1、MTI448版本 打包测试版。 2、光智版本 修改用户手册 上传时间：2022年12月8日14:13:05
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="287">
   <si>
     <t>使用公司</t>
   </si>
@@ -2043,16 +2043,26 @@
   <si>
     <t>图库新增涂鸦，文字，分析（分析未做）</t>
   </si>
+  <si>
+    <t>2022年12月8日14:10:46</t>
+  </si>
+  <si>
+    <t>1.5.02</t>
+  </si>
+  <si>
+    <t>1、MTI448版本 打包测试版。
+2、光智版本 修改用户手册</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -2123,6 +2133,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -2131,14 +2149,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2153,16 +2179,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2174,9 +2201,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2191,16 +2241,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2208,46 +2257,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2261,7 +2271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2288,13 +2298,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2306,43 +2352,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2360,19 +2382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2384,13 +2400,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2402,19 +2466,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2426,49 +2478,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2534,7 +2544,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2558,7 +2568,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2578,17 +2603,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2604,26 +2618,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2635,10 +2645,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2647,133 +2657,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3626,8 +3636,8 @@
   <sheetPr/>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
@@ -21656,10 +21666,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.625" defaultRowHeight="60" customHeight="1"/>
@@ -22268,6 +22278,20 @@
       </c>
       <c r="D47" s="2" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="48" customHeight="1" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" s="1">
+        <v>252</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
分支：dyt_targetApi31_0825 版本：VersionName:1.5.03 ,VersionCode:253 1、可见文档 doc/readme_close_release.txt 2、版本信息：进出图库加限制，对于资源释放有带调整。 上传时间：2022年12月10日11:20:51
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="295">
   <si>
     <t>使用公司</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>VzLMFTlCwp0XolRLl4+ZbA==</t>
+  </si>
+  <si>
+    <t>MTI448(精明鼠)</t>
+  </si>
+  <si>
+    <t>DYTMT448</t>
   </si>
   <si>
     <t>软件包名</t>
@@ -2053,15 +2059,33 @@
     <t>1、MTI448版本 打包测试版。
 2、光智版本 修改用户手册</t>
   </si>
+  <si>
+    <t>2022年12月9日17:08:04</t>
+  </si>
+  <si>
+    <t>1.5.03</t>
+  </si>
+  <si>
+    <t>修改jni对于close release资料释放的闪退问题。存在一个A/libc: FORTIFY: pthread_mutex_lock called on a destroyed mutex (0xb400007601df89a4)</t>
+  </si>
+  <si>
+    <t>2022年12月9日17:40:42</t>
+  </si>
+  <si>
+    <t>1.5.04</t>
+  </si>
+  <si>
+    <t>多次调用mUvcCameraHandler.close();</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31">
@@ -2133,18 +2157,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2155,9 +2179,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2172,24 +2218,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2203,7 +2234,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2217,6 +2248,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -2224,15 +2271,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2248,32 +2293,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2298,7 +2322,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2310,7 +2334,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2322,31 +2406,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2364,73 +2484,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2442,43 +2502,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2544,6 +2568,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2560,15 +2593,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2620,20 +2644,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2645,10 +2669,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2657,7 +2681,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2666,124 +2690,124 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3636,8 +3660,8 @@
   <sheetPr/>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
@@ -4839,11 +4863,19 @@
       <c r="S41" s="19"/>
     </row>
     <row r="42" customHeight="1" spans="1:19">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
+      <c r="A42" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>115</v>
+      </c>
       <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
+      <c r="D42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
@@ -4982,8 +5014,9 @@
       <c r="S48" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H42:L42"/>
     <mergeCell ref="H16:L18"/>
     <mergeCell ref="H2:L7"/>
     <mergeCell ref="H21:L22"/>
@@ -5020,22 +5053,22 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -5049,22 +5082,22 @@
     </row>
     <row r="2" customHeight="1" spans="1:16384">
       <c r="A2" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -21447,179 +21480,179 @@
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" ht="39" customHeight="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" ht="41" customHeight="1" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" ht="31" customHeight="1" spans="1:6">
       <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>159</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>157</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" ht="45" customHeight="1" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="20"/>
@@ -21642,7 +21675,7 @@
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E18" s="20"/>
     </row>
@@ -21666,10 +21699,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.625" defaultRowHeight="60" customHeight="1"/>
@@ -21682,14 +21715,14 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -21697,16 +21730,16 @@
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
@@ -21714,15 +21747,15 @@
     </row>
     <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -21731,40 +21764,40 @@
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" customHeight="1" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E6" s="8"/>
     </row>
@@ -21784,93 +21817,93 @@
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" customHeight="1" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E11" s="8"/>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E12" s="8"/>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E13" s="8"/>
     </row>
     <row r="14" customHeight="1" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" customHeight="1" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -21882,58 +21915,58 @@
     </row>
     <row r="17" customHeight="1" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E17" s="8"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E18" s="8"/>
     </row>
     <row r="19" customHeight="1" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E19" s="8"/>
     </row>
     <row r="20" customHeight="1" spans="1:9">
       <c r="A20" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B20" s="8">
         <v>101</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -21942,356 +21975,384 @@
     </row>
     <row r="21" customHeight="1" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B21" s="8">
         <v>102</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
       <c r="A22" s="8" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B22" s="8">
         <v>103</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E22" s="8"/>
     </row>
     <row r="23" customHeight="1" spans="1:5">
       <c r="A23" s="8" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B23" s="8">
         <v>104</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E23" s="8"/>
     </row>
     <row r="24" ht="122" customHeight="1" spans="1:5">
       <c r="A24" s="8" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B24" s="8">
         <v>105</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E24" s="12"/>
     </row>
     <row r="25" ht="90" customHeight="1" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2">
         <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B27" s="1">
         <v>113</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B28" s="1">
         <v>201</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B29" s="1">
         <v>203</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B30" s="1">
         <v>204</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B31" s="1">
         <v>205</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B32" s="1">
         <v>206</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B33" s="1">
         <v>207</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" ht="88" customHeight="1" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B34" s="1">
         <v>208</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" ht="151" customHeight="1" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B35" s="1">
         <v>209</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" ht="101" customHeight="1" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B36" s="1">
         <v>216</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" ht="134" customHeight="1" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B37" s="1">
         <v>217</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" ht="77" customHeight="1"/>
     <row r="41" customHeight="1" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2">
         <v>232</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E41" s="2"/>
     </row>
     <row r="42" customHeight="1" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" customHeight="1" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B43" s="2">
         <v>233</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E43" s="2"/>
     </row>
     <row r="44" customHeight="1" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B44" s="2">
         <v>234</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" customHeight="1" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B45" s="1">
         <v>235</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B47" s="1">
         <v>251</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B48" s="1">
         <v>252</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" customHeight="1" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" s="1">
+        <v>253</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" customHeight="1" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50" s="1">
+        <v>254</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
分支：dyt_targetApi31_0825 版本：VersionName:1.5.10 ,VersionCode:260 去除所有版本manifest bugly和软件内升级所声明的多余权限 上传时间：2023年1月12日11:33:23
</commit_message>
<xml_diff>
--- a/app/点扬H2F项目分支详情合表.xlsx
+++ b/app/点扬H2F项目分支详情合表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="28125" windowHeight="12540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SN区分表" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="301">
   <si>
     <t>使用公司</t>
   </si>
@@ -2086,14 +2086,24 @@
   <si>
     <t>debug版</t>
   </si>
+  <si>
+    <t>2023年1月9日17:56:15</t>
+  </si>
+  <si>
+    <t>1.5.10</t>
+  </si>
+  <si>
+    <t>1、泰视朗、迈测 MTI256I版本打包apk、迈测，泰视朗打包aab 上架谷歌（所有分支都去除bugly的引用）。
+2、修改“用户手册”权限闪退的问题。所有分支去除“用户手册” assets 目录的拷贝，所有的文件拷贝放在 app/.../main/ui/PreviewActivity.java 当中</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -2159,10 +2169,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2173,32 +2184,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2219,15 +2221,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -2235,7 +2261,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -2250,30 +2276,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -2290,7 +2300,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2324,7 +2334,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2336,13 +2400,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2354,13 +2412,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2372,13 +2430,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2390,19 +2454,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2414,31 +2472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2450,19 +2484,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2474,13 +2502,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2492,19 +2514,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2576,16 +2586,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2606,16 +2616,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2646,20 +2656,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2671,10 +2681,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2683,133 +2693,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3659,7 +3669,7 @@
   <sheetPr/>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -21689,16 +21699,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.625" defaultRowHeight="60" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="26.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.8833333333333" style="2" customWidth="1"/>
+    <col min="4" max="4" width="65.725" style="2" customWidth="1"/>
     <col min="5" max="5" width="62.4916666666667" style="3" customWidth="1"/>
     <col min="6" max="16384" width="26.625" style="3" customWidth="1"/>
   </cols>
@@ -22391,6 +22403,20 @@
       </c>
       <c r="E53" s="3" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="54" customHeight="1" spans="1:4">
+      <c r="A54" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B54" s="1">
+        <v>260</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>